<commit_message>
Report interactions User in Excel
</commit_message>
<xml_diff>
--- a/MyProject2/Content/Excels/Reports.xlsx
+++ b/MyProject2/Content/Excels/Reports.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="34">
   <si>
     <t>nombre</t>
   </si>
@@ -110,13 +110,31 @@
   </si>
   <si>
     <t>Engineering</t>
+  </si>
+  <si>
+    <t>User1</t>
+  </si>
+  <si>
+    <t>CEO</t>
+  </si>
+  <si>
+    <t>Soft</t>
+  </si>
+  <si>
+    <t>contactame@gmail.com</t>
+  </si>
+  <si>
+    <t>Hard</t>
+  </si>
+  <si>
+    <t/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="7">
+  <numFmts count="9">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd\ h:mm:ss"/>
     <numFmt numFmtId="165" formatCode="yyyy-mm-dd h:mm:ss"/>
     <numFmt numFmtId="166" formatCode="yyyy-mm-dd h:mm:ss"/>
@@ -124,6 +142,8 @@
     <numFmt numFmtId="168" formatCode="yyyy-mm-dd h:mm:ss"/>
     <numFmt numFmtId="169" formatCode="yyyy-mm-dd h:mm:ss"/>
     <numFmt numFmtId="170" formatCode="yyyy-mm-dd h:mm:ss"/>
+    <numFmt numFmtId="171" formatCode="yyyy-mm-dd h:mm:ss"/>
+    <numFmt numFmtId="172" formatCode="yyyy-mm-dd h:mm:ss"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="0">
     <font>
@@ -204,7 +224,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFill="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -232,6 +252,8 @@
     <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" applyNumberFormat="1"/>
+    <xf numFmtId="172" fontId="0" fillId="0" borderId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -827,7 +849,7 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J1"/>
+  <dimension ref="A1:J3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G10" sqref="G10"/>
@@ -862,6 +884,52 @@
       </c>
       <c r="J1" s="1" t="s">
         <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10">
+      <c r="D2" s="19">
+        <v>44172.6333333333</v>
+      </c>
+      <c r="E2" t="s">
+        <v>28</v>
+      </c>
+      <c r="F2" t="s">
+        <v>26</v>
+      </c>
+      <c r="G2" t="s">
+        <v>27</v>
+      </c>
+      <c r="H2" t="s">
+        <v>29</v>
+      </c>
+      <c r="I2" t="s">
+        <v>30</v>
+      </c>
+      <c r="J2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10">
+      <c r="D3" s="20">
+        <v>44172.6333333333</v>
+      </c>
+      <c r="E3" t="s">
+        <v>28</v>
+      </c>
+      <c r="F3" t="s">
+        <v>26</v>
+      </c>
+      <c r="G3" t="s">
+        <v>27</v>
+      </c>
+      <c r="H3" t="s">
+        <v>29</v>
+      </c>
+      <c r="I3" t="s">
+        <v>32</v>
+      </c>
+      <c r="J3" t="s">
+        <v>33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Llamadas personales working + excel update
</commit_message>
<xml_diff>
--- a/MyProject2/Content/Excels/Reports.xlsx
+++ b/MyProject2/Content/Excels/Reports.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23426"/>
   <workbookPr/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ivan\Desktop\Secpholand\MyProject2\Content\Excels\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88844C05-31C5-4390-A2BC-E95B87C67C65}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView activeTab="1" xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240"/>
+    <workbookView xWindow="-28920" yWindow="1995" windowWidth="29040" windowHeight="15840" firstSheet="2" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Conexiones Dias + Mapa" sheetId="1" r:id="rId1"/>
@@ -18,15 +19,15 @@
     <sheet name="Inscritos a evento" sheetId="4" r:id="rId4"/>
     <sheet name="Listado de progresion" sheetId="5" r:id="rId5"/>
     <sheet name="informe ausentes" sheetId="6" r:id="rId6"/>
-    <sheet name="informe interaccion stand" sheetId="7" r:id="rId7"/>
-    <sheet name="informe interaccion" sheetId="8" r:id="rId8"/>
+    <sheet name="informe interaccion" sheetId="8" r:id="rId7"/>
+    <sheet name="informe interaccion stand" sheetId="7" r:id="rId8"/>
   </sheets>
   <calcPr calcId="162913" concurrentCalc="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="35">
   <si>
     <t>nombre</t>
   </si>
@@ -129,23 +130,18 @@
   <si>
     <t/>
   </si>
+  <si>
+    <t>Empresa que pide</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="9">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd\ h:mm:ss"/>
-    <numFmt numFmtId="165" formatCode="yyyy-mm-dd h:mm:ss"/>
-    <numFmt numFmtId="166" formatCode="yyyy-mm-dd h:mm:ss"/>
-    <numFmt numFmtId="167" formatCode="yyyy-mm-dd h:mm:ss"/>
-    <numFmt numFmtId="168" formatCode="yyyy-mm-dd h:mm:ss"/>
-    <numFmt numFmtId="169" formatCode="yyyy-mm-dd h:mm:ss"/>
-    <numFmt numFmtId="170" formatCode="yyyy-mm-dd h:mm:ss"/>
-    <numFmt numFmtId="171" formatCode="yyyy-mm-dd h:mm:ss"/>
-    <numFmt numFmtId="172" formatCode="yyyy-mm-dd h:mm:ss"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="0">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -166,6 +162,14 @@
       <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="20"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
@@ -226,16 +230,16 @@
   </cellStyleXfs>
   <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFill="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFill="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -246,14 +250,14 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" applyNumberFormat="1"/>
-    <xf numFmtId="172" fontId="0" fillId="0" borderId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -263,6 +267,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -530,14 +537,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.14062" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="22.5703125" customWidth="1"/>
     <col min="2" max="2" width="24.42578125" customWidth="1"/>
@@ -572,11 +579,11 @@
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="13">
-        <v>44177.4166666667</v>
-      </c>
-      <c r="B2" s="14">
-        <v>44177.4166666667</v>
+      <c r="A2" s="12">
+        <v>44177.416666666701</v>
+      </c>
+      <c r="B2" s="13">
+        <v>44177.416666666701</v>
       </c>
       <c r="C2" t="s">
         <v>25</v>
@@ -595,11 +602,11 @@
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="15">
-        <v>44177.4166666667</v>
-      </c>
-      <c r="B3" s="16">
-        <v>44177.4166666667</v>
+      <c r="A3" s="14">
+        <v>44177.416666666701</v>
+      </c>
+      <c r="B3" s="15">
+        <v>44177.416666666701</v>
       </c>
       <c r="C3" t="s">
         <v>25</v>
@@ -618,11 +625,11 @@
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="17">
-        <v>44177.4166666667</v>
-      </c>
-      <c r="B4" s="18">
-        <v>44177.4166666667</v>
+      <c r="A4" s="16">
+        <v>44177.416666666701</v>
+      </c>
+      <c r="B4" s="17">
+        <v>44177.416666666701</v>
       </c>
       <c r="C4" t="s">
         <v>25</v>
@@ -647,47 +654,43 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="18.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>7</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="7"/>
-      <c r="B2" s="8"/>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="9"/>
-      <c r="B3" s="10"/>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="11"/>
-      <c r="B4" s="12"/>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="6"/>
+      <c r="B2" s="7"/>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="8"/>
+      <c r="B3" s="9"/>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="10"/>
+      <c r="B4" s="11"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -696,33 +699,27 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:D1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J38" sqref="J38"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>7</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>1</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>3</v>
       </c>
     </row>
   </sheetData>
@@ -731,7 +728,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:F1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -766,7 +763,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:I17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -774,6 +771,9 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="6" max="6" width="15" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
@@ -804,7 +804,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="17" spans="8:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="H17" s="5"/>
     </row>
   </sheetData>
@@ -813,7 +813,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:F1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -848,97 +848,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:10" ht="45" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10">
-      <c r="D2" s="19">
-        <v>44172.6333333333</v>
-      </c>
-      <c r="E2" t="s">
-        <v>28</v>
-      </c>
-      <c r="F2" t="s">
-        <v>26</v>
-      </c>
-      <c r="G2" t="s">
-        <v>27</v>
-      </c>
-      <c r="H2" t="s">
-        <v>29</v>
-      </c>
-      <c r="I2" t="s">
-        <v>30</v>
-      </c>
-      <c r="J2" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10">
-      <c r="D3" s="20">
-        <v>44172.6333333333</v>
-      </c>
-      <c r="E3" t="s">
-        <v>28</v>
-      </c>
-      <c r="F3" t="s">
-        <v>26</v>
-      </c>
-      <c r="G3" t="s">
-        <v>27</v>
-      </c>
-      <c r="H3" t="s">
-        <v>29</v>
-      </c>
-      <c r="I3" t="s">
-        <v>32</v>
-      </c>
-      <c r="J3" t="s">
-        <v>33</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A4:H4"/>
   <sheetViews>
     <sheetView topLeftCell="A4" workbookViewId="0">
@@ -980,4 +890,98 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+  <dimension ref="A1:M3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M1" sqref="M1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:13" ht="47.25" x14ac:dyDescent="0.4">
+      <c r="A1" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="M1" s="20" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="D2" s="18">
+        <v>44172.633333333302</v>
+      </c>
+      <c r="E2" t="s">
+        <v>28</v>
+      </c>
+      <c r="F2" t="s">
+        <v>26</v>
+      </c>
+      <c r="G2" t="s">
+        <v>27</v>
+      </c>
+      <c r="H2" t="s">
+        <v>29</v>
+      </c>
+      <c r="I2" t="s">
+        <v>30</v>
+      </c>
+      <c r="J2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="D3" s="19">
+        <v>44172.633333333302</v>
+      </c>
+      <c r="E3" t="s">
+        <v>28</v>
+      </c>
+      <c r="F3" t="s">
+        <v>26</v>
+      </c>
+      <c r="G3" t="s">
+        <v>27</v>
+      </c>
+      <c r="H3" t="s">
+        <v>29</v>
+      </c>
+      <c r="I3" t="s">
+        <v>32</v>
+      </c>
+      <c r="J3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Report XLS stand EP
</commit_message>
<xml_diff>
--- a/MyProject2/Content/Excels/Reports.xlsx
+++ b/MyProject2/Content/Excels/Reports.xlsx
@@ -152,7 +152,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="31">
+  <numFmts count="33">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd\ h:mm:ss"/>
     <numFmt numFmtId="165" formatCode="yyyy-mm-dd h:mm:ss"/>
     <numFmt numFmtId="166" formatCode="yyyy-mm-dd h:mm:ss"/>
@@ -184,6 +184,8 @@
     <numFmt numFmtId="192" formatCode="yyyy-mm-dd h:mm:ss"/>
     <numFmt numFmtId="193" formatCode="yyyy-mm-dd h:mm:ss"/>
     <numFmt numFmtId="194" formatCode="yyyy-mm-dd h:mm:ss"/>
+    <numFmt numFmtId="195" formatCode="yyyy-mm-dd h:mm:ss"/>
+    <numFmt numFmtId="196" formatCode="yyyy-mm-dd h:mm:ss"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="0">
     <font>
@@ -272,7 +274,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFill="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -316,8 +318,9 @@
     <xf numFmtId="188" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="190" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="192" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="193" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="194" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="195" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="196" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -929,7 +932,7 @@
       <c r="B2">
         <v>1</v>
       </c>
-      <c r="D2" s="35">
+      <c r="D2" s="36">
         <v>44172.6333333333</v>
       </c>
       <c r="E2" t="s">
@@ -952,7 +955,7 @@
       <c r="B3">
         <v>1</v>
       </c>
-      <c r="D3" s="36">
+      <c r="D3" s="37">
         <v>44172.6333333333</v>
       </c>
       <c r="E3" t="s">

</xml_diff>

<commit_message>
super user reports update
</commit_message>
<xml_diff>
--- a/MyProject2/Content/Excels/Reports.xlsx
+++ b/MyProject2/Content/Excels/Reports.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23426"/>
   <workbookPr/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ivan\Desktop\Secpholand\MyProject2\Content\Excels\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4629EEF-17D8-4509-8CB6-6755F8FDDAAC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView activeTab="6" xWindow="-28920" yWindow="1995" windowWidth="29040" windowHeight="15840"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" firstSheet="1" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Conexiones Dias + Mapa" sheetId="1" r:id="rId1"/>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="37">
   <si>
     <t>nombre</t>
   </si>
@@ -133,16 +134,7 @@
     <t>Empresa que pide</t>
   </si>
   <si>
-    <t>Scientific investigation</t>
-  </si>
-  <si>
     <t>Kiosco</t>
-  </si>
-  <si>
-    <t>None</t>
-  </si>
-  <si>
-    <t>Classe Usuario MAX</t>
   </si>
   <si>
     <t>Ofertas trabajo</t>
@@ -151,43 +143,11 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="33">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd\ h:mm:ss"/>
-    <numFmt numFmtId="165" formatCode="yyyy-mm-dd h:mm:ss"/>
-    <numFmt numFmtId="166" formatCode="yyyy-mm-dd h:mm:ss"/>
-    <numFmt numFmtId="167" formatCode="yyyy-mm-dd h:mm:ss"/>
-    <numFmt numFmtId="168" formatCode="yyyy-mm-dd h:mm:ss"/>
-    <numFmt numFmtId="169" formatCode="yyyy-mm-dd h:mm:ss"/>
-    <numFmt numFmtId="170" formatCode="yyyy-mm-dd h:mm:ss"/>
-    <numFmt numFmtId="171" formatCode="yyyy-mm-dd h:mm:ss"/>
-    <numFmt numFmtId="172" formatCode="yyyy-mm-dd h:mm:ss"/>
-    <numFmt numFmtId="173" formatCode="yyyy-mm-dd h:mm:ss"/>
-    <numFmt numFmtId="174" formatCode="yyyy-mm-dd h:mm:ss"/>
-    <numFmt numFmtId="175" formatCode="yyyy-mm-dd h:mm:ss"/>
-    <numFmt numFmtId="176" formatCode="yyyy-mm-dd h:mm:ss"/>
-    <numFmt numFmtId="177" formatCode="yyyy-mm-dd h:mm:ss"/>
-    <numFmt numFmtId="178" formatCode="yyyy-mm-dd h:mm:ss"/>
-    <numFmt numFmtId="179" formatCode="yyyy-mm-dd h:mm:ss"/>
-    <numFmt numFmtId="180" formatCode="yyyy-mm-dd h:mm:ss"/>
-    <numFmt numFmtId="181" formatCode="yyyy-mm-dd h:mm:ss"/>
-    <numFmt numFmtId="182" formatCode="yyyy-mm-dd h:mm:ss"/>
-    <numFmt numFmtId="183" formatCode="yyyy-mm-dd h:mm:ss"/>
-    <numFmt numFmtId="184" formatCode="yyyy-mm-dd h:mm:ss"/>
-    <numFmt numFmtId="185" formatCode="yyyy-mm-dd h:mm:ss"/>
-    <numFmt numFmtId="186" formatCode="yyyy-mm-dd h:mm:ss"/>
-    <numFmt numFmtId="187" formatCode="yyyy-mm-dd h:mm:ss"/>
-    <numFmt numFmtId="188" formatCode="yyyy-mm-dd h:mm:ss"/>
-    <numFmt numFmtId="189" formatCode="yyyy-mm-dd h:mm:ss"/>
-    <numFmt numFmtId="190" formatCode="yyyy-mm-dd h:mm:ss"/>
-    <numFmt numFmtId="191" formatCode="yyyy-mm-dd h:mm:ss"/>
-    <numFmt numFmtId="192" formatCode="yyyy-mm-dd h:mm:ss"/>
-    <numFmt numFmtId="193" formatCode="yyyy-mm-dd h:mm:ss"/>
-    <numFmt numFmtId="194" formatCode="yyyy-mm-dd h:mm:ss"/>
-    <numFmt numFmtId="195" formatCode="yyyy-mm-dd h:mm:ss"/>
-    <numFmt numFmtId="196" formatCode="yyyy-mm-dd h:mm:ss"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="0">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -274,18 +234,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFill="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFill="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -304,23 +264,8 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="172" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="174" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="180" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="182" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="184" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="186" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="188" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="190" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="192" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="194" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="195" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="196" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -330,6 +275,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -597,14 +545,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+      <selection activeCell="B1" sqref="B1:B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.14062" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="22.5703125" customWidth="1"/>
     <col min="2" max="2" width="24.42578125" customWidth="1"/>
@@ -640,7 +588,7 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B2" s="13">
         <v>1</v>
@@ -663,7 +611,7 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="14" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B3" s="15">
         <v>1</v>
@@ -686,10 +634,10 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="16">
-        <v>44177.4166666667</v>
+        <v>44177.416666666701</v>
       </c>
       <c r="B4" s="17">
-        <v>44177.4166666667</v>
+        <v>44177.416666666701</v>
       </c>
       <c r="C4" t="s">
         <v>25</v>
@@ -714,7 +662,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -723,11 +671,10 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="18.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>7</v>
       </c>
@@ -760,7 +707,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:D1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -769,7 +716,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:4" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>7</v>
       </c>
@@ -789,7 +736,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:F1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -824,7 +771,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:I17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -836,7 +783,7 @@
     <col min="6" max="6" width="15" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -865,7 +812,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="17" spans="8:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="H17" s="5"/>
     </row>
   </sheetData>
@@ -874,7 +821,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:F1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -909,11 +856,11 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:H4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+  <dimension ref="A1:H3"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -925,15 +872,38 @@
     <col min="8" max="8" width="41.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:8">
+    <row r="1" spans="1:8" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B2">
         <v>1</v>
       </c>
-      <c r="D2" s="36">
-        <v>44172.6333333333</v>
+      <c r="D2" s="21">
+        <v>44172.633333333302</v>
       </c>
       <c r="E2" t="s">
         <v>28</v>
@@ -945,18 +915,18 @@
         <v>27</v>
       </c>
       <c r="H2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="3" spans="1:8">
-      <c r="A3" t="s">
-        <v>39</v>
-      </c>
       <c r="B3">
         <v>1</v>
       </c>
-      <c r="D3" s="37">
-        <v>44172.6333333333</v>
+      <c r="D3" s="22">
+        <v>44172.633333333302</v>
       </c>
       <c r="E3" t="s">
         <v>28</v>
@@ -968,30 +938,7 @@
         <v>27</v>
       </c>
       <c r="H3" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="H4" s="1" t="s">
-        <v>21</v>
+        <v>36</v>
       </c>
     </row>
   </sheetData>
@@ -1000,11 +947,11 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:M3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M1" sqref="M1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1043,7 +990,7 @@
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="D2" s="18">
-        <v>44172.6333333333</v>
+        <v>44172.633333333302</v>
       </c>
       <c r="E2" t="s">
         <v>28</v>
@@ -1066,7 +1013,7 @@
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="D3" s="19">
-        <v>44172.6333333333</v>
+        <v>44172.633333333302</v>
       </c>
       <c r="E3" t="s">
         <v>28</v>

</xml_diff>

<commit_message>
Update File of Excel
</commit_message>
<xml_diff>
--- a/MyProject2/Content/Excels/Reports.xlsx
+++ b/MyProject2/Content/Excels/Reports.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23426"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ivan\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86F73E9F-BD2F-4216-AA57-39638E7DB20D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView activeTab="3" xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240"/>
   </bookViews>
   <sheets>
     <sheet name="Conexiones Dias + Mapa" sheetId="1" r:id="rId1"/>
@@ -27,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="315" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="325" uniqueCount="81">
   <si>
     <t>nombre</t>
   </si>
@@ -261,16 +260,60 @@
   </si>
   <si>
     <t>Hora de inscripción</t>
+  </si>
+  <si>
+    <t>prueba</t>
+  </si>
+  <si>
+    <t>Cluster Manager</t>
+  </si>
+  <si>
+    <t>Producer</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="36">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd\ h:mm:ss"/>
+    <numFmt numFmtId="165" formatCode="yyyy-mm-dd h:mm:ss"/>
+    <numFmt numFmtId="166" formatCode="yyyy-mm-dd h:mm:ss"/>
+    <numFmt numFmtId="167" formatCode="yyyy-mm-dd h:mm:ss"/>
+    <numFmt numFmtId="168" formatCode="yyyy-mm-dd h:mm:ss"/>
+    <numFmt numFmtId="169" formatCode="yyyy-mm-dd h:mm:ss"/>
+    <numFmt numFmtId="170" formatCode="yyyy-mm-dd h:mm:ss"/>
+    <numFmt numFmtId="171" formatCode="yyyy-mm-dd h:mm:ss"/>
+    <numFmt numFmtId="172" formatCode="yyyy-mm-dd h:mm:ss"/>
+    <numFmt numFmtId="173" formatCode="yyyy-mm-dd h:mm:ss"/>
+    <numFmt numFmtId="174" formatCode="yyyy-mm-dd h:mm:ss"/>
+    <numFmt numFmtId="175" formatCode="yyyy-mm-dd h:mm:ss"/>
+    <numFmt numFmtId="176" formatCode="yyyy-mm-dd h:mm:ss"/>
+    <numFmt numFmtId="177" formatCode="yyyy-mm-dd h:mm:ss"/>
+    <numFmt numFmtId="178" formatCode="yyyy-mm-dd h:mm:ss"/>
+    <numFmt numFmtId="179" formatCode="yyyy-mm-dd h:mm:ss"/>
+    <numFmt numFmtId="180" formatCode="yyyy-mm-dd h:mm:ss"/>
+    <numFmt numFmtId="181" formatCode="yyyy-mm-dd h:mm:ss"/>
+    <numFmt numFmtId="182" formatCode="yyyy-mm-dd h:mm:ss"/>
+    <numFmt numFmtId="183" formatCode="yyyy-mm-dd h:mm:ss"/>
+    <numFmt numFmtId="184" formatCode="yyyy-mm-dd h:mm:ss"/>
+    <numFmt numFmtId="185" formatCode="yyyy-mm-dd h:mm:ss"/>
+    <numFmt numFmtId="186" formatCode="yyyy-mm-dd h:mm:ss"/>
+    <numFmt numFmtId="187" formatCode="yyyy-mm-dd h:mm:ss"/>
+    <numFmt numFmtId="188" formatCode="yyyy-mm-dd h:mm:ss"/>
+    <numFmt numFmtId="189" formatCode="yyyy-mm-dd h:mm:ss"/>
+    <numFmt numFmtId="190" formatCode="yyyy-mm-dd h:mm:ss"/>
+    <numFmt numFmtId="191" formatCode="yyyy-mm-dd h:mm:ss"/>
+    <numFmt numFmtId="192" formatCode="yyyy-mm-dd h:mm:ss"/>
+    <numFmt numFmtId="193" formatCode="yyyy-mm-dd h:mm:ss"/>
+    <numFmt numFmtId="194" formatCode="yyyy-mm-dd h:mm:ss"/>
+    <numFmt numFmtId="195" formatCode="yyyy-mm-dd h:mm:ss"/>
+    <numFmt numFmtId="196" formatCode="yyyy-mm-dd h:mm:ss"/>
+    <numFmt numFmtId="197" formatCode="yyyy-mm-dd h:mm:ss"/>
+    <numFmt numFmtId="198" formatCode="yyyy-mm-dd h:mm:ss"/>
+    <numFmt numFmtId="199" formatCode="yyyy-mm-dd h:mm:ss"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="0">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -350,18 +393,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="65">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFill="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFill="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -389,6 +432,41 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="172" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="173" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="174" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="175" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="180" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="181" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="182" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="183" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="184" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="185" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="186" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="187" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="188" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="189" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="190" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="191" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="192" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="193" fontId="0" fillId="0" borderId="0" applyNumberFormat="1"/>
+    <xf numFmtId="194" fontId="0" fillId="0" borderId="0" applyNumberFormat="1"/>
+    <xf numFmtId="195" fontId="0" fillId="0" borderId="0" applyNumberFormat="1"/>
+    <xf numFmtId="196" fontId="0" fillId="0" borderId="0" applyNumberFormat="1"/>
+    <xf numFmtId="197" fontId="0" fillId="0" borderId="0" applyNumberFormat="1"/>
+    <xf numFmtId="198" fontId="0" fillId="0" borderId="0" applyNumberFormat="1"/>
+    <xf numFmtId="199" fontId="0" fillId="0" borderId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -398,9 +476,6 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -668,14 +743,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.14062" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="22.5703125" customWidth="1"/>
     <col min="2" max="2" width="24.42578125" customWidth="1"/>
@@ -711,7 +786,7 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="6">
-        <v>44180.416666666701</v>
+        <v>44180.4166666667</v>
       </c>
       <c r="B2" s="7">
         <v>44180.5</v>
@@ -737,7 +812,7 @@
         <v>44175.5</v>
       </c>
       <c r="B3" s="9">
-        <v>44175.591666666704</v>
+        <v>44175.5916666667</v>
       </c>
       <c r="C3" t="s">
         <v>41</v>
@@ -762,7 +837,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -771,10 +846,11 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>7</v>
       </c>
@@ -791,11 +867,11 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="24">
-        <v>44180.416666666701</v>
-      </c>
-      <c r="B2" s="25">
+    <row r="2" spans="1:5">
+      <c r="A2" s="52">
+        <v>44180.4166666667</v>
+      </c>
+      <c r="B2" s="53">
         <v>44180.5</v>
       </c>
       <c r="C2" t="s">
@@ -804,12 +880,15 @@
       <c r="D2" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="26">
-        <v>44175.083333333299</v>
-      </c>
-      <c r="B3" s="27">
+      <c r="E2" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" s="54">
+        <v>44175.0833333333</v>
+      </c>
+      <c r="B3" s="55">
         <v>44175.125</v>
       </c>
       <c r="C3" t="s">
@@ -818,18 +897,24 @@
       <c r="D3" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="28">
-        <v>44119.166666666701</v>
-      </c>
-      <c r="B4" s="29">
+      <c r="E3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" s="56">
+        <v>44119.1666666667</v>
+      </c>
+      <c r="B4" s="57">
         <v>44119.5</v>
       </c>
       <c r="C4" t="s">
         <v>27</v>
       </c>
       <c r="D4" t="s">
+        <v>27</v>
+      </c>
+      <c r="E4" t="s">
         <v>27</v>
       </c>
     </row>
@@ -840,7 +925,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -879,7 +964,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="11">
-        <v>44175.166666666701</v>
+        <v>44175.1666666667</v>
       </c>
       <c r="B3" t="s">
         <v>57</v>
@@ -891,7 +976,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
@@ -908,7 +993,7 @@
     <col min="8" max="8" width="22.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" ht="45.75" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -934,7 +1019,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8">
       <c r="A2" t="s">
         <v>37</v>
       </c>
@@ -953,8 +1038,14 @@
       <c r="F2" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G2" t="s">
+        <v>26</v>
+      </c>
+      <c r="H2" s="58">
+        <v>44181.5326388889</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
       <c r="A3" t="s">
         <v>59</v>
       </c>
@@ -973,8 +1064,14 @@
       <c r="F3" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G3" t="s">
+        <v>79</v>
+      </c>
+      <c r="H3" s="59">
+        <v>44181.5326388889</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
       <c r="A4" t="s">
         <v>50</v>
       </c>
@@ -993,8 +1090,14 @@
       <c r="F4" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G4" t="s">
+        <v>27</v>
+      </c>
+      <c r="H4" s="60">
+        <v>44181.5326388889</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
       <c r="A5" t="s">
         <v>52</v>
       </c>
@@ -1013,8 +1116,14 @@
       <c r="F5" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G5" t="s">
+        <v>27</v>
+      </c>
+      <c r="H5" s="61">
+        <v>44181.5326388889</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
       <c r="A6" t="s">
         <v>61</v>
       </c>
@@ -1033,8 +1142,14 @@
       <c r="F6" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G6" t="s">
+        <v>80</v>
+      </c>
+      <c r="H6" s="62">
+        <v>44181.5326388889</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
       <c r="A7" t="s">
         <v>56</v>
       </c>
@@ -1053,8 +1168,14 @@
       <c r="F7" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G7" t="s">
+        <v>78</v>
+      </c>
+      <c r="H7" s="63">
+        <v>44181.5326388889</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8">
       <c r="A8" t="s">
         <v>41</v>
       </c>
@@ -1072,6 +1193,12 @@
       </c>
       <c r="F8" t="s">
         <v>38</v>
+      </c>
+      <c r="G8" t="s">
+        <v>34</v>
+      </c>
+      <c r="H8" s="64">
+        <v>44181.5326388889</v>
       </c>
     </row>
   </sheetData>
@@ -1080,7 +1207,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1562,7 +1689,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1737,7 +1864,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1784,7 +1911,7 @@
         <v>1</v>
       </c>
       <c r="D2" s="19">
-        <v>44172.633333333302</v>
+        <v>44172.6333333333</v>
       </c>
       <c r="E2" t="s">
         <v>37</v>
@@ -1807,7 +1934,7 @@
         <v>1</v>
       </c>
       <c r="D3" s="20">
-        <v>44172.633333333302</v>
+        <v>44172.6333333333</v>
       </c>
       <c r="E3" t="s">
         <v>37</v>
@@ -1828,7 +1955,7 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1877,7 +2004,7 @@
         <v>3</v>
       </c>
       <c r="D2" s="21">
-        <v>44168.559027777803</v>
+        <v>44168.5590277778</v>
       </c>
       <c r="E2" t="s">
         <v>37</v>
@@ -1900,7 +2027,7 @@
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="D3" s="22">
-        <v>44175.668749999997</v>
+        <v>44175.66875</v>
       </c>
       <c r="E3" t="s">
         <v>54</v>
@@ -1923,7 +2050,7 @@
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="D4" s="23">
-        <v>44174.565277777801</v>
+        <v>44174.5652777778</v>
       </c>
       <c r="E4" t="s">
         <v>41</v>

</xml_diff>

<commit_message>
1. cambios ready for 0.6.4
</commit_message>
<xml_diff>
--- a/MyProject2/Content/Excels/Reports.xlsx
+++ b/MyProject2/Content/Excels/Reports.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23716"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23530"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ivan\Desktop\Secpholand\MyProject2\Content\Excels\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A9306EF9-09B5-4C94-810B-526EE1EB152D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D72046B3-0FAC-4A87-97BA-3C9415A30E2D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" firstSheet="7" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Conexiones Dias + Mapa" sheetId="1" r:id="rId1"/>
@@ -22,23 +22,12 @@
     <sheet name="informe interaccion" sheetId="8" r:id="rId7"/>
     <sheet name="informe interaccion stand" sheetId="7" r:id="rId8"/>
   </sheets>
-  <calcPr calcId="191028" calcCompleted="0" concurrentCalc="0"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <calcPr calcId="191028" concurrentCalc="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="321" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="318" uniqueCount="83">
   <si>
     <t>Fecha in</t>
   </si>
@@ -89,9 +78,6 @@
   </si>
   <si>
     <t>Cargo</t>
-  </si>
-  <si>
-    <t>Pedro Carrillo</t>
   </si>
   <si>
     <t>prueba</t>
@@ -299,7 +285,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd\ h:mm:ss"/>
   </numFmts>
-  <fonts count="3">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -681,7 +667,7 @@
       <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="22.5703125" customWidth="1"/>
     <col min="2" max="2" width="24.42578125" customWidth="1"/>
@@ -692,7 +678,7 @@
     <col min="7" max="7" width="36.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -715,7 +701,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="6">
         <v>44180.416666666701</v>
       </c>
@@ -738,7 +724,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="6">
         <v>44175.5</v>
       </c>
@@ -769,18 +755,18 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:E1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="18.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>14</v>
       </c>
@@ -795,23 +781,6 @@
       </c>
       <c r="E1" s="1" t="s">
         <v>16</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5">
-      <c r="A2" s="6">
-        <v>44180.416666666701</v>
-      </c>
-      <c r="B2" s="6">
-        <v>44180.5</v>
-      </c>
-      <c r="C2" t="s">
-        <v>17</v>
-      </c>
-      <c r="D2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E2" t="s">
-        <v>18</v>
       </c>
     </row>
   </sheetData>
@@ -828,9 +797,9 @@
       <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>14</v>
       </c>
@@ -844,7 +813,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="6">
         <v>44175.5</v>
       </c>
@@ -858,12 +827,12 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="6">
         <v>44175.166666666701</v>
       </c>
       <c r="B3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
   </sheetData>
@@ -875,11 +844,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:J8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J1" sqref="J1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="19.140625" customWidth="1"/>
     <col min="4" max="4" width="27.5703125" customWidth="1"/>
@@ -889,7 +858,7 @@
     <col min="8" max="8" width="22.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="30">
+    <row r="1" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>2</v>
       </c>
@@ -903,155 +872,155 @@
         <v>5</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>20</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>21</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>16</v>
       </c>
       <c r="H1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="J1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="2" spans="1:10">
-      <c r="A2" t="s">
-        <v>25</v>
-      </c>
       <c r="B2" t="s">
         <v>8</v>
       </c>
       <c r="C2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D2" t="s">
         <v>9</v>
       </c>
       <c r="E2" t="s">
+        <v>26</v>
+      </c>
+      <c r="F2" t="s">
         <v>27</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>28</v>
-      </c>
-      <c r="G2" t="s">
-        <v>29</v>
       </c>
       <c r="H2" s="6">
         <v>44181.532638888901</v>
       </c>
     </row>
-    <row r="3" spans="1:10">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3" t="s">
         <v>30</v>
       </c>
-      <c r="B3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3" t="s">
-        <v>26</v>
-      </c>
-      <c r="D3" t="s">
-        <v>13</v>
-      </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
+        <v>25</v>
+      </c>
+      <c r="G3" t="s">
         <v>31</v>
-      </c>
-      <c r="F3" t="s">
-        <v>26</v>
-      </c>
-      <c r="G3" t="s">
-        <v>32</v>
       </c>
       <c r="H3" s="6">
         <v>44181.532638888901</v>
       </c>
     </row>
-    <row r="4" spans="1:10">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>32</v>
+      </c>
+      <c r="B4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" t="s">
+        <v>25</v>
+      </c>
+      <c r="D4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4" t="s">
         <v>33</v>
       </c>
-      <c r="B4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" t="s">
-        <v>26</v>
-      </c>
-      <c r="D4" t="s">
-        <v>13</v>
-      </c>
-      <c r="E4" t="s">
+      <c r="F4" t="s">
+        <v>25</v>
+      </c>
+      <c r="G4" t="s">
         <v>34</v>
-      </c>
-      <c r="F4" t="s">
-        <v>26</v>
-      </c>
-      <c r="G4" t="s">
-        <v>35</v>
       </c>
       <c r="H4" s="6">
         <v>44181.532638888901</v>
       </c>
     </row>
-    <row r="5" spans="1:10">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>35</v>
+      </c>
+      <c r="B5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" t="s">
+        <v>25</v>
+      </c>
+      <c r="D5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E5" t="s">
         <v>36</v>
       </c>
-      <c r="B5" t="s">
-        <v>8</v>
-      </c>
-      <c r="C5" t="s">
-        <v>26</v>
-      </c>
-      <c r="D5" t="s">
-        <v>13</v>
-      </c>
-      <c r="E5" t="s">
-        <v>37</v>
-      </c>
       <c r="F5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="H5" s="6">
         <v>44181.532638888901</v>
       </c>
     </row>
-    <row r="6" spans="1:10">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>37</v>
+      </c>
+      <c r="B6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" t="s">
+        <v>25</v>
+      </c>
+      <c r="D6" t="s">
+        <v>13</v>
+      </c>
+      <c r="E6" t="s">
         <v>38</v>
       </c>
-      <c r="B6" t="s">
-        <v>8</v>
-      </c>
-      <c r="C6" t="s">
-        <v>26</v>
-      </c>
-      <c r="D6" t="s">
-        <v>13</v>
-      </c>
-      <c r="E6" t="s">
+      <c r="F6" t="s">
+        <v>25</v>
+      </c>
+      <c r="G6" t="s">
         <v>39</v>
-      </c>
-      <c r="F6" t="s">
-        <v>26</v>
-      </c>
-      <c r="G6" t="s">
-        <v>40</v>
       </c>
       <c r="H6" s="6">
         <v>44181.532638888901</v>
       </c>
     </row>
-    <row r="7" spans="1:10">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -1059,25 +1028,25 @@
         <v>8</v>
       </c>
       <c r="C7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D7" t="s">
         <v>9</v>
       </c>
       <c r="E7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="H7" s="6">
         <v>44181.532638888901</v>
       </c>
     </row>
-    <row r="8" spans="1:10">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>11</v>
       </c>
@@ -1085,19 +1054,19 @@
         <v>12</v>
       </c>
       <c r="C8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D8" t="s">
         <v>13</v>
       </c>
       <c r="E8" t="s">
+        <v>41</v>
+      </c>
+      <c r="F8" t="s">
+        <v>25</v>
+      </c>
+      <c r="G8" t="s">
         <v>42</v>
-      </c>
-      <c r="F8" t="s">
-        <v>26</v>
-      </c>
-      <c r="G8" t="s">
-        <v>43</v>
       </c>
       <c r="H8" s="6">
         <v>44181.532638888901</v>
@@ -1116,12 +1085,12 @@
       <selection activeCell="I25" sqref="I25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="6" max="6" width="15" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="30">
+    <row r="1" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>2</v>
       </c>
@@ -1135,51 +1104,51 @@
         <v>5</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="I1" s="1" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9">
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B2" t="s">
         <v>8</v>
       </c>
       <c r="C2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D2" t="s">
         <v>9</v>
       </c>
       <c r="E2" t="s">
+        <v>48</v>
+      </c>
+      <c r="F2" t="s">
         <v>49</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>50</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>51</v>
       </c>
-      <c r="H2" t="s">
-        <v>52</v>
-      </c>
       <c r="I2" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -1187,347 +1156,347 @@
         <v>8</v>
       </c>
       <c r="C3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D3" t="s">
         <v>9</v>
       </c>
       <c r="E3" t="s">
+        <v>52</v>
+      </c>
+      <c r="F3" t="s">
+        <v>52</v>
+      </c>
+      <c r="G3" t="s">
+        <v>50</v>
+      </c>
+      <c r="H3" t="s">
+        <v>51</v>
+      </c>
+      <c r="I3" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>53</v>
       </c>
-      <c r="F3" t="s">
-        <v>53</v>
-      </c>
-      <c r="G3" t="s">
-        <v>51</v>
-      </c>
-      <c r="H3" t="s">
-        <v>52</v>
-      </c>
-      <c r="I3" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9">
-      <c r="A4" t="s">
-        <v>54</v>
-      </c>
       <c r="B4" t="s">
         <v>8</v>
       </c>
       <c r="C4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D4" t="s">
         <v>9</v>
       </c>
       <c r="E4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G4" t="s">
+        <v>54</v>
+      </c>
+      <c r="H4" t="s">
+        <v>51</v>
+      </c>
+      <c r="I4" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>37</v>
+      </c>
+      <c r="B5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" t="s">
+        <v>25</v>
+      </c>
+      <c r="D5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E5" t="s">
+        <v>48</v>
+      </c>
+      <c r="F5" t="s">
+        <v>48</v>
+      </c>
+      <c r="G5" t="s">
         <v>55</v>
       </c>
-      <c r="H4" t="s">
-        <v>52</v>
-      </c>
-      <c r="I4" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9">
-      <c r="A5" t="s">
-        <v>38</v>
-      </c>
-      <c r="B5" t="s">
-        <v>8</v>
-      </c>
-      <c r="C5" t="s">
-        <v>26</v>
-      </c>
-      <c r="D5" t="s">
-        <v>13</v>
-      </c>
-      <c r="E5" t="s">
-        <v>49</v>
-      </c>
-      <c r="F5" t="s">
-        <v>49</v>
-      </c>
-      <c r="G5" t="s">
+      <c r="H5" t="s">
+        <v>51</v>
+      </c>
+      <c r="I5" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>29</v>
+      </c>
+      <c r="B6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" t="s">
+        <v>25</v>
+      </c>
+      <c r="D6" t="s">
+        <v>13</v>
+      </c>
+      <c r="E6" t="s">
+        <v>48</v>
+      </c>
+      <c r="F6" t="s">
+        <v>48</v>
+      </c>
+      <c r="G6" t="s">
+        <v>54</v>
+      </c>
+      <c r="H6" t="s">
+        <v>51</v>
+      </c>
+      <c r="I6" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>56</v>
       </c>
-      <c r="H5" t="s">
-        <v>52</v>
-      </c>
-      <c r="I5" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9">
-      <c r="A6" t="s">
-        <v>30</v>
-      </c>
-      <c r="B6" t="s">
-        <v>8</v>
-      </c>
-      <c r="C6" t="s">
-        <v>26</v>
-      </c>
-      <c r="D6" t="s">
-        <v>13</v>
-      </c>
-      <c r="E6" t="s">
-        <v>49</v>
-      </c>
-      <c r="F6" t="s">
-        <v>49</v>
-      </c>
-      <c r="G6" t="s">
-        <v>55</v>
-      </c>
-      <c r="H6" t="s">
-        <v>52</v>
-      </c>
-      <c r="I6" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9">
-      <c r="A7" t="s">
+      <c r="B7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" t="s">
+        <v>25</v>
+      </c>
+      <c r="D7" t="s">
+        <v>13</v>
+      </c>
+      <c r="E7" t="s">
+        <v>52</v>
+      </c>
+      <c r="F7" t="s">
+        <v>52</v>
+      </c>
+      <c r="G7" t="s">
+        <v>51</v>
+      </c>
+      <c r="H7" t="s">
+        <v>51</v>
+      </c>
+      <c r="I7" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
         <v>57</v>
       </c>
-      <c r="B7" t="s">
-        <v>8</v>
-      </c>
-      <c r="C7" t="s">
-        <v>26</v>
-      </c>
-      <c r="D7" t="s">
-        <v>13</v>
-      </c>
-      <c r="E7" t="s">
-        <v>53</v>
-      </c>
-      <c r="F7" t="s">
-        <v>53</v>
-      </c>
-      <c r="G7" t="s">
-        <v>52</v>
-      </c>
-      <c r="H7" t="s">
-        <v>52</v>
-      </c>
-      <c r="I7" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9">
-      <c r="A8" t="s">
+      <c r="B8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8" t="s">
+        <v>25</v>
+      </c>
+      <c r="D8" t="s">
+        <v>13</v>
+      </c>
+      <c r="E8" t="s">
+        <v>48</v>
+      </c>
+      <c r="F8" t="s">
+        <v>48</v>
+      </c>
+      <c r="G8" t="s">
+        <v>51</v>
+      </c>
+      <c r="H8" t="s">
+        <v>51</v>
+      </c>
+      <c r="I8" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>32</v>
+      </c>
+      <c r="B9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C9" t="s">
+        <v>25</v>
+      </c>
+      <c r="D9" t="s">
+        <v>13</v>
+      </c>
+      <c r="E9" t="s">
+        <v>48</v>
+      </c>
+      <c r="F9" t="s">
+        <v>48</v>
+      </c>
+      <c r="G9" t="s">
+        <v>51</v>
+      </c>
+      <c r="H9" t="s">
+        <v>51</v>
+      </c>
+      <c r="I9" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>35</v>
+      </c>
+      <c r="B10" t="s">
+        <v>8</v>
+      </c>
+      <c r="C10" t="s">
+        <v>25</v>
+      </c>
+      <c r="D10" t="s">
+        <v>13</v>
+      </c>
+      <c r="E10" t="s">
+        <v>48</v>
+      </c>
+      <c r="F10" t="s">
+        <v>48</v>
+      </c>
+      <c r="G10" t="s">
+        <v>51</v>
+      </c>
+      <c r="H10" t="s">
+        <v>51</v>
+      </c>
+      <c r="I10" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
         <v>58</v>
       </c>
-      <c r="B8" t="s">
-        <v>8</v>
-      </c>
-      <c r="C8" t="s">
-        <v>26</v>
-      </c>
-      <c r="D8" t="s">
-        <v>13</v>
-      </c>
-      <c r="E8" t="s">
-        <v>49</v>
-      </c>
-      <c r="F8" t="s">
-        <v>49</v>
-      </c>
-      <c r="G8" t="s">
-        <v>52</v>
-      </c>
-      <c r="H8" t="s">
-        <v>52</v>
-      </c>
-      <c r="I8" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9">
-      <c r="A9" t="s">
-        <v>33</v>
-      </c>
-      <c r="B9" t="s">
-        <v>8</v>
-      </c>
-      <c r="C9" t="s">
-        <v>26</v>
-      </c>
-      <c r="D9" t="s">
-        <v>13</v>
-      </c>
-      <c r="E9" t="s">
-        <v>49</v>
-      </c>
-      <c r="F9" t="s">
-        <v>49</v>
-      </c>
-      <c r="G9" t="s">
-        <v>52</v>
-      </c>
-      <c r="H9" t="s">
-        <v>52</v>
-      </c>
-      <c r="I9" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9">
-      <c r="A10" t="s">
-        <v>36</v>
-      </c>
-      <c r="B10" t="s">
-        <v>8</v>
-      </c>
-      <c r="C10" t="s">
-        <v>26</v>
-      </c>
-      <c r="D10" t="s">
-        <v>13</v>
-      </c>
-      <c r="E10" t="s">
-        <v>49</v>
-      </c>
-      <c r="F10" t="s">
-        <v>49</v>
-      </c>
-      <c r="G10" t="s">
-        <v>52</v>
-      </c>
-      <c r="H10" t="s">
-        <v>52</v>
-      </c>
-      <c r="I10" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9">
-      <c r="A11" t="s">
+      <c r="B11" t="s">
+        <v>8</v>
+      </c>
+      <c r="C11" t="s">
+        <v>25</v>
+      </c>
+      <c r="D11" t="s">
         <v>59</v>
       </c>
-      <c r="B11" t="s">
-        <v>8</v>
-      </c>
-      <c r="C11" t="s">
-        <v>26</v>
-      </c>
-      <c r="D11" t="s">
+      <c r="E11" t="s">
+        <v>48</v>
+      </c>
+      <c r="F11" t="s">
+        <v>48</v>
+      </c>
+      <c r="G11" t="s">
         <v>60</v>
       </c>
-      <c r="E11" t="s">
-        <v>49</v>
-      </c>
-      <c r="F11" t="s">
-        <v>49</v>
-      </c>
-      <c r="G11" t="s">
+      <c r="H11" t="s">
+        <v>51</v>
+      </c>
+      <c r="I11" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
         <v>61</v>
       </c>
-      <c r="H11" t="s">
-        <v>52</v>
-      </c>
-      <c r="I11" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9">
-      <c r="A12" t="s">
+      <c r="B12" t="s">
+        <v>8</v>
+      </c>
+      <c r="C12" t="s">
+        <v>25</v>
+      </c>
+      <c r="D12" t="s">
         <v>62</v>
       </c>
-      <c r="B12" t="s">
-        <v>8</v>
-      </c>
-      <c r="C12" t="s">
-        <v>26</v>
-      </c>
-      <c r="D12" t="s">
+      <c r="E12" t="s">
+        <v>48</v>
+      </c>
+      <c r="F12" t="s">
+        <v>48</v>
+      </c>
+      <c r="G12" t="s">
+        <v>51</v>
+      </c>
+      <c r="H12" t="s">
+        <v>51</v>
+      </c>
+      <c r="I12" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
         <v>63</v>
       </c>
-      <c r="E12" t="s">
-        <v>49</v>
-      </c>
-      <c r="F12" t="s">
-        <v>49</v>
-      </c>
-      <c r="G12" t="s">
-        <v>52</v>
-      </c>
-      <c r="H12" t="s">
-        <v>52</v>
-      </c>
-      <c r="I12" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9">
-      <c r="A13" t="s">
-        <v>64</v>
-      </c>
       <c r="B13" t="s">
         <v>8</v>
       </c>
       <c r="C13" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D13" t="s">
         <v>9</v>
       </c>
       <c r="E13" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F13" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G13" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="H13" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="I13" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B14" t="s">
         <v>8</v>
       </c>
       <c r="C14" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D14" t="s">
         <v>9</v>
       </c>
       <c r="E14" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F14" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G14" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="H14" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="I14" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>11</v>
       </c>
@@ -1535,54 +1504,54 @@
         <v>12</v>
       </c>
       <c r="C15" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D15" t="s">
         <v>13</v>
       </c>
       <c r="E15" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F15" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G15" t="s">
+        <v>50</v>
+      </c>
+      <c r="H15" t="s">
         <v>51</v>
       </c>
-      <c r="H15" t="s">
-        <v>52</v>
-      </c>
       <c r="I15" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B16" t="s">
         <v>12</v>
       </c>
       <c r="C16" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D16" t="s">
         <v>13</v>
       </c>
       <c r="E16" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F16" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="G16" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="H16" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="I16" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
   </sheetData>
@@ -1598,11 +1567,11 @@
       <selection sqref="A1:F1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:6" ht="30">
+    <row r="1" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>2</v>
@@ -1617,10 +1586,10 @@
         <v>5</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="6">
         <v>44109</v>
       </c>
@@ -1631,133 +1600,133 @@
         <v>12</v>
       </c>
       <c r="D2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E2" t="s">
         <v>13</v>
       </c>
       <c r="F2" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="6">
         <v>44102</v>
       </c>
       <c r="B3" t="s">
+        <v>61</v>
+      </c>
+      <c r="C3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" t="s">
+        <v>25</v>
+      </c>
+      <c r="E3" t="s">
         <v>62</v>
       </c>
-      <c r="C3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D3" t="s">
-        <v>26</v>
-      </c>
-      <c r="E3" t="s">
-        <v>63</v>
-      </c>
       <c r="F3" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="6">
         <v>44099</v>
       </c>
       <c r="B4" t="s">
+        <v>58</v>
+      </c>
+      <c r="C4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" t="s">
+        <v>25</v>
+      </c>
+      <c r="E4" t="s">
         <v>59</v>
       </c>
-      <c r="C4" t="s">
-        <v>8</v>
-      </c>
-      <c r="D4" t="s">
-        <v>26</v>
-      </c>
-      <c r="E4" t="s">
-        <v>60</v>
-      </c>
       <c r="F4" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="6">
         <v>44099</v>
       </c>
       <c r="B5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C5" t="s">
         <v>8</v>
       </c>
       <c r="D5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E5" t="s">
         <v>13</v>
       </c>
       <c r="F5" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="6">
         <v>44099</v>
       </c>
       <c r="B6" t="s">
+        <v>32</v>
+      </c>
+      <c r="C6" t="s">
+        <v>8</v>
+      </c>
+      <c r="D6" t="s">
+        <v>25</v>
+      </c>
+      <c r="E6" t="s">
+        <v>13</v>
+      </c>
+      <c r="F6" t="s">
         <v>33</v>
       </c>
-      <c r="C6" t="s">
-        <v>8</v>
-      </c>
-      <c r="D6" t="s">
-        <v>26</v>
-      </c>
-      <c r="E6" t="s">
-        <v>13</v>
-      </c>
-      <c r="F6" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6">
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="6">
         <v>44099</v>
       </c>
       <c r="B7" t="s">
+        <v>35</v>
+      </c>
+      <c r="C7" t="s">
+        <v>8</v>
+      </c>
+      <c r="D7" t="s">
+        <v>25</v>
+      </c>
+      <c r="E7" t="s">
+        <v>13</v>
+      </c>
+      <c r="F7" t="s">
         <v>36</v>
       </c>
-      <c r="C7" t="s">
-        <v>8</v>
-      </c>
-      <c r="D7" t="s">
-        <v>26</v>
-      </c>
-      <c r="E7" t="s">
-        <v>13</v>
-      </c>
-      <c r="F7" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6">
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="6">
         <v>44096</v>
       </c>
       <c r="B8" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C8" t="s">
         <v>8</v>
       </c>
       <c r="D8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E8" t="s">
         <v>13</v>
       </c>
       <c r="F8" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
   </sheetData>
@@ -1773,7 +1742,7 @@
       <selection activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="4" max="4" width="24.140625" customWidth="1"/>
     <col min="5" max="5" width="16.7109375" customWidth="1"/>
@@ -1782,15 +1751,15 @@
     <col min="8" max="8" width="41.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="30">
+    <row r="1" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="D1" s="4" t="s">
         <v>74</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>75</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>2</v>
@@ -1802,12 +1771,12 @@
         <v>5</v>
       </c>
       <c r="H1" s="1" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>76</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8">
-      <c r="A2" t="s">
-        <v>77</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -1816,7 +1785,7 @@
         <v>44172.633333333302</v>
       </c>
       <c r="E2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F2" t="s">
         <v>8</v>
@@ -1825,12 +1794,12 @@
         <v>9</v>
       </c>
       <c r="H2" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>77</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8">
-      <c r="A3" t="s">
-        <v>78</v>
       </c>
       <c r="B3">
         <v>1</v>
@@ -1839,7 +1808,7 @@
         <v>44172.633333333302</v>
       </c>
       <c r="E3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F3" t="s">
         <v>8</v>
@@ -1848,7 +1817,7 @@
         <v>9</v>
       </c>
       <c r="H3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
   </sheetData>
@@ -1864,20 +1833,20 @@
       <selection activeCell="K9" sqref="K9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="4" max="4" width="18.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="47.25">
+    <row r="1" spans="1:13" ht="47.25" x14ac:dyDescent="0.4">
       <c r="A1" s="4" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="D1" s="4" t="s">
         <v>74</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>75</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>2</v>
@@ -1892,18 +1861,18 @@
         <v>16</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="J1" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="M1" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>80</v>
-      </c>
-      <c r="M1" s="5" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13">
-      <c r="A2" t="s">
-        <v>81</v>
       </c>
       <c r="B2">
         <v>3</v>
@@ -1912,7 +1881,7 @@
         <v>44168.559027777803</v>
       </c>
       <c r="E2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F2" t="s">
         <v>8</v>
@@ -1921,21 +1890,21 @@
         <v>9</v>
       </c>
       <c r="H2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="I2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="J2" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="D3" s="6">
         <v>44175.668749999997</v>
       </c>
       <c r="E3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F3" t="s">
         <v>8</v>
@@ -1944,18 +1913,18 @@
         <v>13</v>
       </c>
       <c r="H3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="I3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="J3" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="D4" s="6">
-        <v>44174.56527777778</v>
+        <v>44174.565277777801</v>
       </c>
       <c r="E4" t="s">
         <v>11</v>
@@ -1967,13 +1936,13 @@
         <v>13</v>
       </c>
       <c r="H4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="I4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="J4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Stand and report Update
</commit_message>
<xml_diff>
--- a/MyProject2/Content/Excels/Reports.xlsx
+++ b/MyProject2/Content/Excels/Reports.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23530"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ivan\Desktop\Secpholand\MyProject2\Content\Excels\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D72046B3-0FAC-4A87-97BA-3C9415A30E2D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView activeTab="6" xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240"/>
   </bookViews>
   <sheets>
     <sheet name="Conexiones Dias + Mapa" sheetId="1" r:id="rId1"/>
@@ -27,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="318" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="384" uniqueCount="98">
   <si>
     <t>Fecha in</t>
   </si>
@@ -266,26 +265,95 @@
     <t>Elemento de stand</t>
   </si>
   <si>
-    <t>Contacto dado?</t>
-  </si>
-  <si>
     <t>Stand1</t>
   </si>
   <si>
     <t>Design Manager</t>
   </si>
   <si>
-    <t>Contactame@gmail.com</t>
+    <t>producto1</t>
+  </si>
+  <si>
+    <t>Interacciones con elementos del stand</t>
+  </si>
+  <si>
+    <t>Tarjetas dejadas</t>
+  </si>
+  <si>
+    <t>User1</t>
+  </si>
+  <si>
+    <t>addie05l_y517q@deypo.com</t>
+  </si>
+  <si>
+    <t>Stand3</t>
+  </si>
+  <si>
+    <t>Stand 5</t>
+  </si>
+  <si>
+    <t>Stand 6</t>
+  </si>
+  <si>
+    <t>Goberto Calleja</t>
+  </si>
+  <si>
+    <t>Guillermo Esteban</t>
+  </si>
+  <si>
+    <t>Carla Barceló</t>
+  </si>
+  <si>
+    <t>Pedro Carrillo</t>
+  </si>
+  <si>
+    <t>Juan Camilla</t>
+  </si>
+  <si>
+    <t>None</t>
+  </si>
+  <si>
+    <t>User3</t>
+  </si>
+  <si>
+    <t>user3@gmail.com</t>
+  </si>
+  <si>
+    <t>User2</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="25">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd\ h:mm:ss"/>
+    <numFmt numFmtId="165" formatCode="yyyy-mm-dd h:mm:ss"/>
+    <numFmt numFmtId="166" formatCode="yyyy-mm-dd h:mm:ss"/>
+    <numFmt numFmtId="167" formatCode="yyyy-mm-dd h:mm:ss"/>
+    <numFmt numFmtId="168" formatCode="yyyy-mm-dd h:mm:ss"/>
+    <numFmt numFmtId="169" formatCode="yyyy-mm-dd h:mm:ss"/>
+    <numFmt numFmtId="170" formatCode="yyyy-mm-dd h:mm:ss"/>
+    <numFmt numFmtId="171" formatCode="yyyy-mm-dd h:mm:ss"/>
+    <numFmt numFmtId="172" formatCode="yyyy-mm-dd h:mm:ss"/>
+    <numFmt numFmtId="173" formatCode="yyyy-mm-dd h:mm:ss"/>
+    <numFmt numFmtId="174" formatCode="yyyy-mm-dd h:mm:ss"/>
+    <numFmt numFmtId="175" formatCode="yyyy-mm-dd h:mm:ss"/>
+    <numFmt numFmtId="176" formatCode="yyyy-mm-dd h:mm:ss"/>
+    <numFmt numFmtId="177" formatCode="yyyy-mm-dd h:mm:ss"/>
+    <numFmt numFmtId="178" formatCode="yyyy-mm-dd h:mm:ss"/>
+    <numFmt numFmtId="179" formatCode="yyyy-mm-dd h:mm:ss"/>
+    <numFmt numFmtId="180" formatCode="yyyy-mm-dd h:mm:ss"/>
+    <numFmt numFmtId="181" formatCode="yyyy-mm-dd h:mm:ss"/>
+    <numFmt numFmtId="182" formatCode="yyyy-mm-dd h:mm:ss"/>
+    <numFmt numFmtId="183" formatCode="yyyy-mm-dd h:mm:ss"/>
+    <numFmt numFmtId="184" formatCode="yyyy-mm-dd h:mm:ss"/>
+    <numFmt numFmtId="185" formatCode="yyyy-mm-dd h:mm:ss"/>
+    <numFmt numFmtId="186" formatCode="yyyy-mm-dd h:mm:ss"/>
+    <numFmt numFmtId="187" formatCode="yyyy-mm-dd h:mm:ss"/>
+    <numFmt numFmtId="188" formatCode="yyyy-mm-dd h:mm:ss"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="0">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -301,8 +369,15 @@
       <family val="2"/>
     </font>
     <font>
+      <sz val="26"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
-      <sz val="20"/>
+      <sz val="26"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -323,7 +398,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -361,26 +436,69 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFill="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFill="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFill="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="172" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="173" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="174" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="175" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="180" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="181" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="182" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="183" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="184" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="185" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="186" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="187" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="188" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -390,9 +508,6 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -660,14 +775,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.14062" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="22.5703125" customWidth="1"/>
     <col min="2" max="2" width="24.42578125" customWidth="1"/>
@@ -702,10 +817,10 @@
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="6">
-        <v>44180.416666666701</v>
-      </c>
-      <c r="B2" s="6">
+      <c r="A2" s="5">
+        <v>44180.4166666667</v>
+      </c>
+      <c r="B2" s="5">
         <v>44180.5</v>
       </c>
       <c r="C2" t="s">
@@ -725,11 +840,11 @@
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="6">
+      <c r="A3" s="5">
         <v>44175.5</v>
       </c>
-      <c r="B3" s="6">
-        <v>44175.591666666704</v>
+      <c r="B3" s="5">
+        <v>44175.5916666667</v>
       </c>
       <c r="C3" t="s">
         <v>11</v>
@@ -754,16 +869,17 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H21" sqref="H21"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.4258" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -790,14 +906,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.4258" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
@@ -814,7 +930,7 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="6">
+      <c r="A2" s="5">
         <v>44175.5</v>
       </c>
       <c r="B2" t="s">
@@ -828,8 +944,8 @@
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="6">
-        <v>44175.166666666701</v>
+      <c r="A3" s="5">
+        <v>44175.1666666667</v>
       </c>
       <c r="B3" t="s">
         <v>18</v>
@@ -841,14 +957,14 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="J1" sqref="J1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.4258" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="19.140625" customWidth="1"/>
     <col min="4" max="4" width="27.5703125" customWidth="1"/>
@@ -912,8 +1028,8 @@
       <c r="G2" t="s">
         <v>28</v>
       </c>
-      <c r="H2" s="6">
-        <v>44181.532638888901</v>
+      <c r="H2" s="5">
+        <v>44181.5326388889</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
@@ -938,8 +1054,8 @@
       <c r="G3" t="s">
         <v>31</v>
       </c>
-      <c r="H3" s="6">
-        <v>44181.532638888901</v>
+      <c r="H3" s="5">
+        <v>44181.5326388889</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
@@ -964,8 +1080,8 @@
       <c r="G4" t="s">
         <v>34</v>
       </c>
-      <c r="H4" s="6">
-        <v>44181.532638888901</v>
+      <c r="H4" s="5">
+        <v>44181.5326388889</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
@@ -990,8 +1106,8 @@
       <c r="G5" t="s">
         <v>34</v>
       </c>
-      <c r="H5" s="6">
-        <v>44181.532638888901</v>
+      <c r="H5" s="5">
+        <v>44181.5326388889</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
@@ -1016,8 +1132,8 @@
       <c r="G6" t="s">
         <v>39</v>
       </c>
-      <c r="H6" s="6">
-        <v>44181.532638888901</v>
+      <c r="H6" s="5">
+        <v>44181.5326388889</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
@@ -1042,8 +1158,8 @@
       <c r="G7" t="s">
         <v>17</v>
       </c>
-      <c r="H7" s="6">
-        <v>44181.532638888901</v>
+      <c r="H7" s="5">
+        <v>44181.5326388889</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
@@ -1068,8 +1184,8 @@
       <c r="G8" t="s">
         <v>42</v>
       </c>
-      <c r="H8" s="6">
-        <v>44181.532638888901</v>
+      <c r="H8" s="5">
+        <v>44181.5326388889</v>
       </c>
     </row>
   </sheetData>
@@ -1078,14 +1194,14 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="I25" sqref="I25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.4258" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="6" max="6" width="15" customWidth="1"/>
   </cols>
@@ -1560,14 +1676,14 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:F1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.4258" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
@@ -1590,7 +1706,7 @@
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="6">
+      <c r="A2" s="5">
         <v>44109</v>
       </c>
       <c r="B2" t="s">
@@ -1610,7 +1726,7 @@
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="6">
+      <c r="A3" s="5">
         <v>44102</v>
       </c>
       <c r="B3" t="s">
@@ -1630,7 +1746,7 @@
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="6">
+      <c r="A4" s="5">
         <v>44099</v>
       </c>
       <c r="B4" t="s">
@@ -1650,7 +1766,7 @@
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="6">
+      <c r="A5" s="5">
         <v>44099</v>
       </c>
       <c r="B5" t="s">
@@ -1670,7 +1786,7 @@
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="6">
+      <c r="A6" s="5">
         <v>44099</v>
       </c>
       <c r="B6" t="s">
@@ -1690,7 +1806,7 @@
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="6">
+      <c r="A7" s="5">
         <v>44099</v>
       </c>
       <c r="B7" t="s">
@@ -1710,7 +1826,7 @@
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="6">
+      <c r="A8" s="5">
         <v>44096</v>
       </c>
       <c r="B8" t="s">
@@ -1735,14 +1851,14 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.4258" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="4" max="4" width="24.140625" customWidth="1"/>
     <col min="5" max="5" width="16.7109375" customWidth="1"/>
@@ -1781,8 +1897,8 @@
       <c r="B2">
         <v>1</v>
       </c>
-      <c r="D2" s="6">
-        <v>44172.633333333302</v>
+      <c r="D2" s="5">
+        <v>44172.6333333333</v>
       </c>
       <c r="E2" t="s">
         <v>24</v>
@@ -1804,8 +1920,8 @@
       <c r="B3">
         <v>1</v>
       </c>
-      <c r="D3" s="6">
-        <v>44172.633333333302</v>
+      <c r="D3" s="5">
+        <v>44172.6333333333</v>
       </c>
       <c r="E3" t="s">
         <v>24</v>
@@ -1826,123 +1942,389 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
-  <dimension ref="A1:M4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:Q14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K9" sqref="K9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.4258" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="71.5703125" customWidth="1"/>
     <col min="4" max="4" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16" customWidth="1"/>
+    <col min="7" max="7" width="23.42578125" customWidth="1"/>
+    <col min="8" max="8" width="23.42578125" customWidth="1"/>
+    <col min="9" max="9" width="26.28515625" customWidth="1"/>
+    <col min="10" max="10" width="24.42578125" customWidth="1"/>
+    <col min="11" max="11" width="32.28515625" customWidth="1"/>
+    <col min="13" max="13" width="29.140625" customWidth="1"/>
+    <col min="14" max="14" width="27" customWidth="1"/>
+    <col min="15" max="15" width="35.28515625" customWidth="1"/>
+    <col min="16" max="16" width="34.42578125" customWidth="1"/>
+    <col min="17" max="17" width="30.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="47.25" x14ac:dyDescent="0.4">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:13" ht="34.5" x14ac:dyDescent="0.55">
+      <c r="A1" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="M1" s="6" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" ht="30.75" x14ac:dyDescent="0.3">
+      <c r="C2" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="F2" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="G2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="H2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="I2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="J2" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="K2" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="M2" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="O2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="P2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q2" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17">
+      <c r="C3" t="s">
         <v>79</v>
       </c>
-      <c r="M1" s="5" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="D3">
+        <v>3</v>
+      </c>
+      <c r="F3" s="21">
+        <v>44168.5590277778</v>
+      </c>
+      <c r="G3" t="s">
+        <v>89</v>
+      </c>
+      <c r="H3" t="s">
+        <v>8</v>
+      </c>
+      <c r="I3" t="s">
+        <v>9</v>
+      </c>
+      <c r="J3" t="s">
+        <v>28</v>
+      </c>
+      <c r="K3" t="s">
+        <v>79</v>
+      </c>
+      <c r="M3" t="s">
+        <v>84</v>
+      </c>
+      <c r="N3" t="s">
+        <v>94</v>
+      </c>
+      <c r="O3" t="s">
+        <v>13</v>
+      </c>
+      <c r="P3" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17">
+      <c r="C4" t="s">
+        <v>86</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="F4" s="22">
+        <v>44174.5652777778</v>
+      </c>
+      <c r="G4" t="s">
+        <v>90</v>
+      </c>
+      <c r="H4" t="s">
+        <v>8</v>
+      </c>
+      <c r="I4" t="s">
+        <v>13</v>
+      </c>
+      <c r="J4" t="s">
+        <v>42</v>
+      </c>
+      <c r="K4" t="s">
+        <v>79</v>
+      </c>
+      <c r="M4" t="s">
+        <v>95</v>
+      </c>
+      <c r="N4" t="s">
+        <v>94</v>
+      </c>
+      <c r="O4" t="s">
+        <v>13</v>
+      </c>
+      <c r="P4" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17">
+      <c r="C5" t="s">
+        <v>87</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="F5" s="23">
+        <v>44175.66875</v>
+      </c>
+      <c r="G5" t="s">
+        <v>91</v>
+      </c>
+      <c r="H5" t="s">
+        <v>8</v>
+      </c>
+      <c r="I5" t="s">
+        <v>13</v>
+      </c>
+      <c r="J5" t="s">
         <v>80</v>
       </c>
-      <c r="B2">
-        <v>3</v>
-      </c>
-      <c r="D2" s="6">
-        <v>44168.559027777803</v>
-      </c>
-      <c r="E2" t="s">
-        <v>24</v>
-      </c>
-      <c r="F2" t="s">
-        <v>8</v>
-      </c>
-      <c r="G2" t="s">
+      <c r="K5" t="s">
+        <v>79</v>
+      </c>
+      <c r="M5" t="s">
+        <v>97</v>
+      </c>
+      <c r="N5" t="s">
+        <v>94</v>
+      </c>
+      <c r="O5" t="s">
+        <v>13</v>
+      </c>
+      <c r="P5" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17">
+      <c r="C6" t="s">
+        <v>88</v>
+      </c>
+      <c r="D6">
+        <v>7</v>
+      </c>
+      <c r="F6" s="24">
+        <v>44182.6923611111</v>
+      </c>
+      <c r="G6" t="s">
+        <v>89</v>
+      </c>
+      <c r="H6" t="s">
+        <v>8</v>
+      </c>
+      <c r="I6" t="s">
         <v>9</v>
       </c>
-      <c r="H2" t="s">
+      <c r="J6" t="s">
         <v>28</v>
       </c>
-      <c r="I2" t="s">
-        <v>80</v>
-      </c>
-      <c r="J2" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="D3" s="6">
-        <v>44175.668749999997</v>
-      </c>
-      <c r="E3" t="s">
-        <v>56</v>
-      </c>
-      <c r="F3" t="s">
-        <v>8</v>
-      </c>
-      <c r="G3" t="s">
-        <v>13</v>
-      </c>
-      <c r="H3" t="s">
-        <v>81</v>
-      </c>
-      <c r="I3" t="s">
-        <v>80</v>
-      </c>
-      <c r="J3" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="D4" s="6">
-        <v>44174.565277777801</v>
-      </c>
-      <c r="E4" t="s">
-        <v>11</v>
-      </c>
-      <c r="F4" t="s">
-        <v>12</v>
-      </c>
-      <c r="G4" t="s">
-        <v>13</v>
-      </c>
-      <c r="H4" t="s">
-        <v>42</v>
-      </c>
-      <c r="I4" t="s">
-        <v>80</v>
-      </c>
-      <c r="J4" t="s">
-        <v>82</v>
+      <c r="K6" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17">
+      <c r="F7" s="25">
+        <v>44230.4423611111</v>
+      </c>
+      <c r="G7" t="s">
+        <v>89</v>
+      </c>
+      <c r="H7" t="s">
+        <v>8</v>
+      </c>
+      <c r="I7" t="s">
+        <v>9</v>
+      </c>
+      <c r="J7" t="s">
+        <v>28</v>
+      </c>
+      <c r="K7" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17">
+      <c r="F8" s="26">
+        <v>44230.4625</v>
+      </c>
+      <c r="G8" t="s">
+        <v>89</v>
+      </c>
+      <c r="H8" t="s">
+        <v>8</v>
+      </c>
+      <c r="I8" t="s">
+        <v>9</v>
+      </c>
+      <c r="J8" t="s">
+        <v>28</v>
+      </c>
+      <c r="K8" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17">
+      <c r="F9" s="27">
+        <v>44230.4673611111</v>
+      </c>
+      <c r="G9" t="s">
+        <v>89</v>
+      </c>
+      <c r="H9" t="s">
+        <v>8</v>
+      </c>
+      <c r="I9" t="s">
+        <v>9</v>
+      </c>
+      <c r="J9" t="s">
+        <v>28</v>
+      </c>
+      <c r="K9" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17">
+      <c r="F10" s="28">
+        <v>44230.6</v>
+      </c>
+      <c r="G10" t="s">
+        <v>92</v>
+      </c>
+      <c r="H10" t="s">
+        <v>8</v>
+      </c>
+      <c r="I10" t="s">
+        <v>9</v>
+      </c>
+      <c r="J10" t="s">
+        <v>17</v>
+      </c>
+      <c r="K10" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17">
+      <c r="F11" s="29">
+        <v>44230.6</v>
+      </c>
+      <c r="G11" t="s">
+        <v>92</v>
+      </c>
+      <c r="H11" t="s">
+        <v>8</v>
+      </c>
+      <c r="I11" t="s">
+        <v>9</v>
+      </c>
+      <c r="J11" t="s">
+        <v>17</v>
+      </c>
+      <c r="K11" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17">
+      <c r="F12" s="30">
+        <v>44230.6</v>
+      </c>
+      <c r="G12" t="s">
+        <v>92</v>
+      </c>
+      <c r="H12" t="s">
+        <v>8</v>
+      </c>
+      <c r="I12" t="s">
+        <v>9</v>
+      </c>
+      <c r="J12" t="s">
+        <v>17</v>
+      </c>
+      <c r="K12" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17">
+      <c r="F13" s="31">
+        <v>44230.6</v>
+      </c>
+      <c r="G13" t="s">
+        <v>93</v>
+      </c>
+      <c r="H13" t="s">
+        <v>8</v>
+      </c>
+      <c r="I13" t="s">
+        <v>9</v>
+      </c>
+      <c r="J13" t="s">
+        <v>17</v>
+      </c>
+      <c r="K13" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17">
+      <c r="F14" s="32">
+        <v>44230.6</v>
+      </c>
+      <c r="G14" t="s">
+        <v>93</v>
+      </c>
+      <c r="H14" t="s">
+        <v>8</v>
+      </c>
+      <c r="I14" t="s">
+        <v>9</v>
+      </c>
+      <c r="J14" t="s">
+        <v>17</v>
+      </c>
+      <c r="K14" t="s">
+        <v>88</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update stand and report
</commit_message>
<xml_diff>
--- a/MyProject2/Content/Excels/Reports.xlsx
+++ b/MyProject2/Content/Excels/Reports.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="384" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="368" uniqueCount="99">
   <si>
     <t>Fecha in</t>
   </si>
@@ -317,13 +317,19 @@
   </si>
   <si>
     <t>User2</t>
+  </si>
+  <si>
+    <t>AsorCAD counter</t>
+  </si>
+  <si>
+    <t>addie05l_y517q@deypo.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="25">
+  <numFmts count="45">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd\ h:mm:ss"/>
     <numFmt numFmtId="165" formatCode="yyyy-mm-dd h:mm:ss"/>
     <numFmt numFmtId="166" formatCode="yyyy-mm-dd h:mm:ss"/>
@@ -349,6 +355,26 @@
     <numFmt numFmtId="186" formatCode="yyyy-mm-dd h:mm:ss"/>
     <numFmt numFmtId="187" formatCode="yyyy-mm-dd h:mm:ss"/>
     <numFmt numFmtId="188" formatCode="yyyy-mm-dd h:mm:ss"/>
+    <numFmt numFmtId="189" formatCode="yyyy-mm-dd h:mm:ss"/>
+    <numFmt numFmtId="190" formatCode="yyyy-mm-dd h:mm:ss"/>
+    <numFmt numFmtId="191" formatCode="yyyy-mm-dd h:mm:ss"/>
+    <numFmt numFmtId="192" formatCode="yyyy-mm-dd h:mm:ss"/>
+    <numFmt numFmtId="193" formatCode="yyyy-mm-dd h:mm:ss"/>
+    <numFmt numFmtId="194" formatCode="yyyy-mm-dd h:mm:ss"/>
+    <numFmt numFmtId="195" formatCode="yyyy-mm-dd h:mm:ss"/>
+    <numFmt numFmtId="196" formatCode="yyyy-mm-dd h:mm:ss"/>
+    <numFmt numFmtId="197" formatCode="yyyy-mm-dd h:mm:ss"/>
+    <numFmt numFmtId="198" formatCode="yyyy-mm-dd h:mm:ss"/>
+    <numFmt numFmtId="199" formatCode="yyyy-mm-dd h:mm:ss"/>
+    <numFmt numFmtId="200" formatCode="yyyy-mm-dd h:mm:ss"/>
+    <numFmt numFmtId="201" formatCode="yyyy-mm-dd h:mm:ss"/>
+    <numFmt numFmtId="202" formatCode="yyyy-mm-dd h:mm:ss"/>
+    <numFmt numFmtId="203" formatCode="yyyy-mm-dd h:mm:ss"/>
+    <numFmt numFmtId="204" formatCode="yyyy-mm-dd h:mm:ss"/>
+    <numFmt numFmtId="205" formatCode="yyyy-mm-dd h:mm:ss"/>
+    <numFmt numFmtId="206" formatCode="yyyy-mm-dd h:mm:ss"/>
+    <numFmt numFmtId="207" formatCode="yyyy-mm-dd h:mm:ss"/>
+    <numFmt numFmtId="208" formatCode="yyyy-mm-dd h:mm:ss"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="0">
     <font>
@@ -452,7 +478,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFill="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -484,18 +510,38 @@
     <xf numFmtId="174" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="175" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyNumberFormat="1"/>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyNumberFormat="1"/>
-    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyNumberFormat="1"/>
-    <xf numFmtId="180" fontId="0" fillId="0" borderId="0" applyNumberFormat="1"/>
-    <xf numFmtId="181" fontId="0" fillId="0" borderId="0" applyNumberFormat="1"/>
-    <xf numFmtId="182" fontId="0" fillId="0" borderId="0" applyNumberFormat="1"/>
-    <xf numFmtId="183" fontId="0" fillId="0" borderId="0" applyNumberFormat="1"/>
-    <xf numFmtId="184" fontId="0" fillId="0" borderId="0" applyNumberFormat="1"/>
-    <xf numFmtId="185" fontId="0" fillId="0" borderId="0" applyNumberFormat="1"/>
-    <xf numFmtId="186" fontId="0" fillId="0" borderId="0" applyNumberFormat="1"/>
-    <xf numFmtId="187" fontId="0" fillId="0" borderId="0" applyNumberFormat="1"/>
-    <xf numFmtId="188" fontId="0" fillId="0" borderId="0" applyNumberFormat="1"/>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="180" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="181" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="182" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="183" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="184" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="185" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="186" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="187" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="188" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="189" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="190" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="191" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="192" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="193" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="194" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="195" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="196" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="197" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="198" fontId="0" fillId="0" borderId="0" applyNumberFormat="1"/>
+    <xf numFmtId="199" fontId="0" fillId="0" borderId="0" applyNumberFormat="1"/>
+    <xf numFmtId="200" fontId="0" fillId="0" borderId="0" applyNumberFormat="1"/>
+    <xf numFmtId="201" fontId="0" fillId="0" borderId="0" applyNumberFormat="1"/>
+    <xf numFmtId="202" fontId="0" fillId="0" borderId="0" applyNumberFormat="1"/>
+    <xf numFmtId="203" fontId="0" fillId="0" borderId="0" applyNumberFormat="1"/>
+    <xf numFmtId="204" fontId="0" fillId="0" borderId="0" applyNumberFormat="1"/>
+    <xf numFmtId="205" fontId="0" fillId="0" borderId="0" applyNumberFormat="1"/>
+    <xf numFmtId="206" fontId="0" fillId="0" borderId="0" applyNumberFormat="1"/>
+    <xf numFmtId="207" fontId="0" fillId="0" borderId="0" applyNumberFormat="1"/>
+    <xf numFmtId="208" fontId="0" fillId="0" borderId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1940,7 +1986,7 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q14"/>
+  <dimension ref="A1:Q13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="F14" sqref="F14"/>
@@ -2017,13 +2063,13 @@
     </row>
     <row r="3" spans="1:17">
       <c r="C3" t="s">
-        <v>79</v>
+        <v>85</v>
       </c>
       <c r="D3">
-        <v>3</v>
-      </c>
-      <c r="F3" s="21">
-        <v>44168.5590277778</v>
+        <v>1</v>
+      </c>
+      <c r="F3" s="42">
+        <v>44230.4423611111</v>
       </c>
       <c r="G3" t="s">
         <v>87</v>
@@ -2038,118 +2084,82 @@
         <v>28</v>
       </c>
       <c r="K3" t="s">
-        <v>79</v>
+        <v>85</v>
       </c>
       <c r="M3" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="N3" t="s">
-        <v>93</v>
+        <v>8</v>
       </c>
       <c r="O3" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="P3" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="Q3" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
     </row>
     <row r="4" spans="1:17">
       <c r="C4" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="D4">
-        <v>1</v>
-      </c>
-      <c r="F4" s="22">
-        <v>44174.5652777778</v>
+        <v>7</v>
+      </c>
+      <c r="F4" s="43">
+        <v>44230.4625</v>
       </c>
       <c r="G4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="H4" t="s">
         <v>8</v>
       </c>
       <c r="I4" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="J4" t="s">
-        <v>42</v>
+        <v>28</v>
       </c>
       <c r="K4" t="s">
-        <v>79</v>
-      </c>
-      <c r="M4" t="s">
-        <v>94</v>
-      </c>
-      <c r="N4" t="s">
-        <v>93</v>
-      </c>
-      <c r="O4" t="s">
-        <v>13</v>
-      </c>
-      <c r="P4" t="s">
-        <v>34</v>
-      </c>
-      <c r="Q4" t="s">
-        <v>95</v>
+        <v>86</v>
       </c>
     </row>
     <row r="5" spans="1:17">
       <c r="C5" t="s">
-        <v>85</v>
+        <v>97</v>
       </c>
       <c r="D5">
-        <v>1</v>
-      </c>
-      <c r="F5" s="23">
-        <v>44175.66875</v>
+        <v>3</v>
+      </c>
+      <c r="F5" s="44">
+        <v>44230.4673611111</v>
       </c>
       <c r="G5" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="H5" t="s">
         <v>8</v>
       </c>
       <c r="I5" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="J5" t="s">
-        <v>80</v>
+        <v>28</v>
       </c>
       <c r="K5" t="s">
-        <v>79</v>
-      </c>
-      <c r="M5" t="s">
-        <v>96</v>
-      </c>
-      <c r="N5" t="s">
-        <v>93</v>
-      </c>
-      <c r="O5" t="s">
-        <v>13</v>
-      </c>
-      <c r="P5" t="s">
-        <v>34</v>
-      </c>
-      <c r="Q5" t="s">
-        <v>40</v>
+        <v>86</v>
       </c>
     </row>
     <row r="6" spans="1:17">
-      <c r="C6" t="s">
-        <v>86</v>
-      </c>
-      <c r="D6">
-        <v>7</v>
-      </c>
-      <c r="F6" s="24">
-        <v>44182.6923611111</v>
+      <c r="F6" s="45">
+        <v>44230.6</v>
       </c>
       <c r="G6" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="H6" t="s">
         <v>8</v>
@@ -2158,18 +2168,18 @@
         <v>9</v>
       </c>
       <c r="J6" t="s">
-        <v>28</v>
+        <v>17</v>
       </c>
       <c r="K6" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
     </row>
     <row r="7" spans="1:17">
-      <c r="F7" s="25">
-        <v>44230.4423611111</v>
+      <c r="F7" s="46">
+        <v>44230.6</v>
       </c>
       <c r="G7" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="H7" t="s">
         <v>8</v>
@@ -2178,18 +2188,18 @@
         <v>9</v>
       </c>
       <c r="J7" t="s">
-        <v>28</v>
+        <v>17</v>
       </c>
       <c r="K7" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
     </row>
     <row r="8" spans="1:17">
-      <c r="F8" s="26">
-        <v>44230.4625</v>
+      <c r="F8" s="47">
+        <v>44230.6</v>
       </c>
       <c r="G8" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="H8" t="s">
         <v>8</v>
@@ -2198,18 +2208,18 @@
         <v>9</v>
       </c>
       <c r="J8" t="s">
-        <v>28</v>
+        <v>17</v>
       </c>
       <c r="K8" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="9" spans="1:17">
-      <c r="F9" s="27">
-        <v>44230.4673611111</v>
+      <c r="F9" s="48">
+        <v>44230.6</v>
       </c>
       <c r="G9" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
       <c r="H9" t="s">
         <v>8</v>
@@ -2218,18 +2228,18 @@
         <v>9</v>
       </c>
       <c r="J9" t="s">
-        <v>28</v>
+        <v>17</v>
       </c>
       <c r="K9" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="10" spans="1:17">
-      <c r="F10" s="28">
+      <c r="F10" s="49">
         <v>44230.6</v>
       </c>
       <c r="G10" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="H10" t="s">
         <v>8</v>
@@ -2245,11 +2255,11 @@
       </c>
     </row>
     <row r="11" spans="1:17">
-      <c r="F11" s="29">
-        <v>44230.6</v>
+      <c r="F11" s="50">
+        <v>44232.5423611111</v>
       </c>
       <c r="G11" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="H11" t="s">
         <v>8</v>
@@ -2258,18 +2268,18 @@
         <v>9</v>
       </c>
       <c r="J11" t="s">
-        <v>17</v>
+        <v>28</v>
       </c>
       <c r="K11" t="s">
-        <v>86</v>
+        <v>97</v>
       </c>
     </row>
     <row r="12" spans="1:17">
-      <c r="F12" s="30">
-        <v>44230.6</v>
+      <c r="F12" s="51">
+        <v>44232.5423611111</v>
       </c>
       <c r="G12" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="H12" t="s">
         <v>8</v>
@@ -2278,18 +2288,18 @@
         <v>9</v>
       </c>
       <c r="J12" t="s">
-        <v>17</v>
+        <v>28</v>
       </c>
       <c r="K12" t="s">
-        <v>86</v>
+        <v>97</v>
       </c>
     </row>
     <row r="13" spans="1:17">
-      <c r="F13" s="31">
-        <v>44230.6</v>
+      <c r="F13" s="52">
+        <v>44232.5444444444</v>
       </c>
       <c r="G13" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="H13" t="s">
         <v>8</v>
@@ -2298,30 +2308,10 @@
         <v>9</v>
       </c>
       <c r="J13" t="s">
-        <v>17</v>
+        <v>28</v>
       </c>
       <c r="K13" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="14" spans="1:17">
-      <c r="F14" s="32">
-        <v>44230.6</v>
-      </c>
-      <c r="G14" t="s">
-        <v>91</v>
-      </c>
-      <c r="H14" t="s">
-        <v>8</v>
-      </c>
-      <c r="I14" t="s">
-        <v>9</v>
-      </c>
-      <c r="J14" t="s">
-        <v>17</v>
-      </c>
-      <c r="K14" t="s">
-        <v>86</v>
+        <v>97</v>
       </c>
     </row>
   </sheetData>

</xml_diff>